<commit_message>
able to record user_data
accuracy need to be reconsidered
</commit_message>
<xml_diff>
--- a/GRE.xlsx
+++ b/GRE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>12b26j</t>
   </si>
@@ -78,9 +78,6 @@
     <t>e2b0tj</t>
   </si>
   <si>
-    <t xml:space="preserve">同义重复 反义重复 </t>
-  </si>
-  <si>
     <t>f2b0sj</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>62b0pj</t>
   </si>
   <si>
-    <t xml:space="preserve">生僻词汇 反义重复 </t>
-  </si>
-  <si>
     <t>22b0oj</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>62b0nj</t>
   </si>
   <si>
-    <t xml:space="preserve">同义重复 </t>
-  </si>
-  <si>
     <t>02b0mj</t>
   </si>
   <si>
@@ -145,6 +136,102 @@
   </si>
   <si>
     <t>生僻词汇 结构复杂 反义重复</t>
+  </si>
+  <si>
+    <t>92b0gj</t>
+  </si>
+  <si>
+    <t>32b0fj</t>
+  </si>
+  <si>
+    <t>42b0ej</t>
+  </si>
+  <si>
+    <t>多次取反 同义重复 生僻词汇</t>
+  </si>
+  <si>
+    <t>22b0dj</t>
+  </si>
+  <si>
+    <t>反义重复 多次取反</t>
+  </si>
+  <si>
+    <t>a2b0cj</t>
+  </si>
+  <si>
+    <t>d2b0bj</t>
+  </si>
+  <si>
+    <t>同义重复 指代关系 生僻词汇</t>
+  </si>
+  <si>
+    <t>52b0aj</t>
+  </si>
+  <si>
+    <t>02b09j</t>
+  </si>
+  <si>
+    <t>同义重复 多次取反 生僻词汇</t>
+  </si>
+  <si>
+    <t>72b08j</t>
+  </si>
+  <si>
+    <t>结构复杂 同义重复</t>
+  </si>
+  <si>
+    <t>62b07j</t>
+  </si>
+  <si>
+    <t>72b06j</t>
+  </si>
+  <si>
+    <t>c2b05j</t>
+  </si>
+  <si>
+    <t>82b04j</t>
+  </si>
+  <si>
+    <t>62b03j</t>
+  </si>
+  <si>
+    <t>多次取反 反义重复 结构复杂</t>
+  </si>
+  <si>
+    <t>92b02j</t>
+  </si>
+  <si>
+    <t>f2b01j</t>
+  </si>
+  <si>
+    <t>02b00j</t>
+  </si>
+  <si>
+    <t>结构复杂 反义重复</t>
+  </si>
+  <si>
+    <t>02azzj</t>
+  </si>
+  <si>
+    <t>结构复杂 熟词僻义 同义重复</t>
+  </si>
+  <si>
+    <t>82azyj</t>
+  </si>
+  <si>
+    <t>反义重复 同义重复 生僻词汇</t>
+  </si>
+  <si>
+    <t>f2azxj</t>
+  </si>
+  <si>
+    <t>结构复杂 多次取反 生僻词汇 同义重复 反义重复</t>
+  </si>
+  <si>
+    <t>同义重复 反义重复</t>
+  </si>
+  <si>
+    <t>生僻词汇 反义重复</t>
   </si>
 </sst>
 </file>
@@ -497,14 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,111 +736,111 @@
         <v>0.74</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.86</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>0.56999999999999995</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>0.66</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0.36</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>0.27</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>0.72</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>0.61</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21">
         <v>0.77</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>0.73</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>0.56000000000000005</v>
@@ -763,35 +851,255 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>0.78</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>0.65</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>0.56000000000000005</v>
       </c>
       <c r="C26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>0.61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>0.75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="B29">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>0.8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>0.86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>0.63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34">
+        <v>0.72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35">
+        <v>0.63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36">
+        <v>0.65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37">
+        <v>0.62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38">
+        <v>0.46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39">
+        <v>0.3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41">
+        <v>0.73</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>0.65</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>0.61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44">
+        <v>0.39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45">
+        <v>0.61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46">
+        <v>0.39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -822,8 +1130,28 @@
     <hyperlink ref="A24" r:id="rId24" display="http://gre.kmf.com/question/12b0ij.html"/>
     <hyperlink ref="A25" r:id="rId25" display="http://gre.kmf.com/question/12b0hj.html"/>
     <hyperlink ref="A26" r:id="rId26" display="http://gre.kmf.com/question/891jwk.html"/>
+    <hyperlink ref="A27" r:id="rId27" display="http://gre.kmf.com/question/92b0gj.html"/>
+    <hyperlink ref="A28" r:id="rId28" display="http://gre.kmf.com/question/32b0fj.html"/>
+    <hyperlink ref="A29" r:id="rId29" display="http://gre.kmf.com/question/42b0ej.html"/>
+    <hyperlink ref="A30" r:id="rId30" display="http://gre.kmf.com/question/22b0dj.html"/>
+    <hyperlink ref="A31" r:id="rId31" display="http://gre.kmf.com/question/a2b0cj.html"/>
+    <hyperlink ref="A32" r:id="rId32" display="http://gre.kmf.com/question/d2b0bj.html"/>
+    <hyperlink ref="A33" r:id="rId33" display="http://gre.kmf.com/question/52b0aj.html"/>
+    <hyperlink ref="A34" r:id="rId34" display="http://gre.kmf.com/question/02b09j.html"/>
+    <hyperlink ref="A35" r:id="rId35" display="http://gre.kmf.com/question/72b08j.html"/>
+    <hyperlink ref="A36" r:id="rId36" display="http://gre.kmf.com/question/62b07j.html"/>
+    <hyperlink ref="A37" r:id="rId37" display="http://gre.kmf.com/question/72b06j.html"/>
+    <hyperlink ref="A38" r:id="rId38" display="http://gre.kmf.com/question/c2b05j.html"/>
+    <hyperlink ref="A39" r:id="rId39" display="http://gre.kmf.com/question/82b04j.html"/>
+    <hyperlink ref="A40" r:id="rId40" display="http://gre.kmf.com/question/62b03j.html"/>
+    <hyperlink ref="A41" r:id="rId41" display="http://gre.kmf.com/question/92b02j.html"/>
+    <hyperlink ref="A42" r:id="rId42" display="http://gre.kmf.com/question/f2b01j.html"/>
+    <hyperlink ref="A43" r:id="rId43" display="http://gre.kmf.com/question/02b00j.html"/>
+    <hyperlink ref="A44" r:id="rId44" display="http://gre.kmf.com/question/02azzj.html"/>
+    <hyperlink ref="A45" r:id="rId45" display="http://gre.kmf.com/question/82azyj.html"/>
+    <hyperlink ref="A46" r:id="rId46" display="http://gre.kmf.com/question/f2azxj.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update GRE tasks set
</commit_message>
<xml_diff>
--- a/GRE.xlsx
+++ b/GRE.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
   <si>
     <t>12b26j</t>
   </si>
@@ -232,13 +233,106 @@
   </si>
   <si>
     <t>生僻词汇 反义重复</t>
+  </si>
+  <si>
+    <t>c2b0wj</t>
+  </si>
+  <si>
+    <t>同义重复 结构复杂</t>
+  </si>
+  <si>
+    <t>82b0xj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">同义重复 生僻词汇 指代关系 </t>
+  </si>
+  <si>
+    <t>72b0yj</t>
+  </si>
+  <si>
+    <t>同义重复 熟词僻义</t>
+  </si>
+  <si>
+    <t>12b0zj</t>
+  </si>
+  <si>
+    <t>12b10j</t>
+  </si>
+  <si>
+    <t>同义重复 生僻词汇 结构复杂 理解困难</t>
+  </si>
+  <si>
+    <t>b2b11j</t>
+  </si>
+  <si>
+    <t>同义重复 理解困难 结构复杂</t>
+  </si>
+  <si>
+    <t>12b12j</t>
+  </si>
+  <si>
+    <t>12b13j</t>
+  </si>
+  <si>
+    <t>理解困难 结构复杂 生僻词汇</t>
+  </si>
+  <si>
+    <t>b2b14j</t>
+  </si>
+  <si>
+    <t>理解困难 熟词僻义 同义重复</t>
+  </si>
+  <si>
+    <t>d2b15j</t>
+  </si>
+  <si>
+    <t>熟词僻义 同义重复 生僻词汇 理解困难</t>
+  </si>
+  <si>
+    <t>d2b16j</t>
+  </si>
+  <si>
+    <t>多次取反 生僻词汇 同义重复</t>
+  </si>
+  <si>
+    <t>82b17j</t>
+  </si>
+  <si>
+    <t>同义重复 反义重复 熟词僻义</t>
+  </si>
+  <si>
+    <t>82b18j</t>
+  </si>
+  <si>
+    <t>同义重复 反义重复 理解困难</t>
+  </si>
+  <si>
+    <t>d2b19j</t>
+  </si>
+  <si>
+    <t>92b1aj</t>
+  </si>
+  <si>
+    <t>22b1bj</t>
+  </si>
+  <si>
+    <t>92b1cj</t>
+  </si>
+  <si>
+    <t>理解困难 结构复杂</t>
+  </si>
+  <si>
+    <t>f2b1dj</t>
+  </si>
+  <si>
+    <t>结构复杂 生僻词汇 理解困难 反义重复</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +355,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -291,18 +409,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,23 +703,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="3" max="3" width="103.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="103.28515625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <v>0.7</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -608,10 +729,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>0.56000000000000005</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -619,10 +740,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.84</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -630,10 +751,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.94</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -641,10 +762,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.81</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -652,10 +773,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.8</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -663,10 +784,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>0.71</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -674,10 +795,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>0.54</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -685,10 +806,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>0.73</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -696,10 +817,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>0.53</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -707,399 +828,597 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>0.74</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>0.74</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>0.86</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>0.66</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>0.36</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>0.27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>0.72</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>0.61</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>0.77</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>0.73</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>0.78</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>0.65</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>0.61</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>0.75</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>0.8</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>0.86</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>0.63</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B33" s="3">
         <v>0.75</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>0.72</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>0.63</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>0.65</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>0.62</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>0.46</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>0.3</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>0.73</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="3">
         <v>0.65</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <v>0.61</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="3">
         <v>0.39</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
         <v>0.61</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>0.39</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1150,8 +1469,26 @@
     <hyperlink ref="A44" r:id="rId44" display="http://gre.kmf.com/question/02azzj.html"/>
     <hyperlink ref="A45" r:id="rId45" display="http://gre.kmf.com/question/82azyj.html"/>
     <hyperlink ref="A46" r:id="rId46" display="http://gre.kmf.com/question/f2azxj.html"/>
+    <hyperlink ref="A47" r:id="rId47" display="http://gre.kmf.com/question/c2b0wj.html"/>
+    <hyperlink ref="A48" r:id="rId48" display="http://gre.kmf.com/question/82b0xj.html"/>
+    <hyperlink ref="A49" r:id="rId49" display="http://gre.kmf.com/question/72b0yj.html"/>
+    <hyperlink ref="A50" r:id="rId50" display="http://gre.kmf.com/question/12b0zj.html"/>
+    <hyperlink ref="A51" r:id="rId51" display="http://gre.kmf.com/question/12b10j.html"/>
+    <hyperlink ref="A52" r:id="rId52" display="http://gre.kmf.com/question/b2b11j.html"/>
+    <hyperlink ref="A53" r:id="rId53" display="http://gre.kmf.com/question/12b12j.html"/>
+    <hyperlink ref="A54" r:id="rId54" display="http://gre.kmf.com/question/12b13j.html"/>
+    <hyperlink ref="A55" r:id="rId55" display="http://gre.kmf.com/question/b2b14j.html"/>
+    <hyperlink ref="A56" r:id="rId56" display="http://gre.kmf.com/question/d2b15j.html"/>
+    <hyperlink ref="A57" r:id="rId57" display="http://gre.kmf.com/question/d2b16j.html"/>
+    <hyperlink ref="A58" r:id="rId58" display="http://gre.kmf.com/question/82b17j.html"/>
+    <hyperlink ref="A59" r:id="rId59" display="http://gre.kmf.com/question/82b18j.html"/>
+    <hyperlink ref="A60" r:id="rId60" display="http://gre.kmf.com/question/d2b19j.html"/>
+    <hyperlink ref="A61" r:id="rId61" display="http://gre.kmf.com/question/92b1aj.html"/>
+    <hyperlink ref="A62" r:id="rId62" display="http://gre.kmf.com/question/22b1bj.html"/>
+    <hyperlink ref="A63" r:id="rId63" display="http://gre.kmf.com/question/92b1cj.html"/>
+    <hyperlink ref="A64" r:id="rId64" display="http://gre.kmf.com/question/f2b1dj.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new GRE verbal task
</commit_message>
<xml_diff>
--- a/GRE.xlsx
+++ b/GRE.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="125">
   <si>
     <t>12b26j</t>
   </si>
@@ -326,6 +325,75 @@
   </si>
   <si>
     <t>结构复杂 生僻词汇 理解困难 反义重复</t>
+  </si>
+  <si>
+    <t>92b1ej</t>
+  </si>
+  <si>
+    <t>结构复杂 同义重复 理解困难</t>
+  </si>
+  <si>
+    <t>22b1fj</t>
+  </si>
+  <si>
+    <t>92b1gj</t>
+  </si>
+  <si>
+    <t>同义重复 反义重复 生僻词汇</t>
+  </si>
+  <si>
+    <t>指代关系  结构复杂 前后倒装</t>
+  </si>
+  <si>
+    <t>02b1hj</t>
+  </si>
+  <si>
+    <t>62b1ij</t>
+  </si>
+  <si>
+    <t>42b1jj</t>
+  </si>
+  <si>
+    <t>82b1kj</t>
+  </si>
+  <si>
+    <t>生僻词汇 反义重复 理解困难</t>
+  </si>
+  <si>
+    <t>62b1lj</t>
+  </si>
+  <si>
+    <t>92b1mj</t>
+  </si>
+  <si>
+    <t>生僻词汇 理解困难 反义重复</t>
+  </si>
+  <si>
+    <t>生僻词汇 理解困难 结构复杂 同义重复 反义重复</t>
+  </si>
+  <si>
+    <t>b2b1nj</t>
+  </si>
+  <si>
+    <t>52b1oj</t>
+  </si>
+  <si>
+    <t>42b1pj</t>
+  </si>
+  <si>
+    <t>同义重复 理解困难</t>
+  </si>
+  <si>
+    <t>62b1qj</t>
+  </si>
+  <si>
+    <t>前后倒装 生僻词汇 反义重复</t>
+  </si>
+  <si>
+    <t>82b1rj</t>
+  </si>
+  <si>
+    <t>反义重复 结构复杂 生僻词汇 指代关系</t>
   </si>
 </sst>
 </file>
@@ -409,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -421,7 +489,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -703,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,7 +1467,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B63" s="3">
@@ -1411,14 +1478,168 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="3">
         <v>0.22</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1487,8 +1708,22 @@
     <hyperlink ref="A62" r:id="rId62" display="http://gre.kmf.com/question/22b1bj.html"/>
     <hyperlink ref="A63" r:id="rId63" display="http://gre.kmf.com/question/92b1cj.html"/>
     <hyperlink ref="A64" r:id="rId64" display="http://gre.kmf.com/question/f2b1dj.html"/>
+    <hyperlink ref="A65" r:id="rId65" display="http://gre.kmf.com/question/92b1ej.html"/>
+    <hyperlink ref="A66" r:id="rId66" display="http://gre.kmf.com/question/22b1fj.html"/>
+    <hyperlink ref="A67" r:id="rId67" display="http://gre.kmf.com/question/92b1gj.html"/>
+    <hyperlink ref="A68" r:id="rId68" display="http://gre.kmf.com/question/02b1hj.html"/>
+    <hyperlink ref="A69" r:id="rId69" display="http://gre.kmf.com/question/62b1ij.html"/>
+    <hyperlink ref="A70" r:id="rId70" display="http://gre.kmf.com/question/42b1jj.html"/>
+    <hyperlink ref="A71" r:id="rId71" display="http://gre.kmf.com/question/82b1kj.html"/>
+    <hyperlink ref="A72" r:id="rId72" display="http://gre.kmf.com/question/62b1lj.html"/>
+    <hyperlink ref="A73" r:id="rId73" display="http://gre.kmf.com/question/92b1mj.html"/>
+    <hyperlink ref="A74" r:id="rId74" display="http://gre.kmf.com/question/b2b1nj.html"/>
+    <hyperlink ref="A75" r:id="rId75" display="http://gre.kmf.com/question/52b1oj.html"/>
+    <hyperlink ref="A76" r:id="rId76" display="http://gre.kmf.com/question/42b1pj.html"/>
+    <hyperlink ref="A77" r:id="rId77" display="http://gre.kmf.com/question/62b1qj.html"/>
+    <hyperlink ref="A78" r:id="rId78" display="http://gre.kmf.com/question/82b1rj.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId65"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId79"/>
 </worksheet>
 </file>
</xml_diff>